<commit_message>
fim da aula 07
</commit_message>
<xml_diff>
--- a/aula_06/notas_alunos.xlsx
+++ b/aula_06/notas_alunos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projetos\ks_1200t15950_\aula_06\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3008D89F-8C90-446C-B943-8BC913BD11A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF47381-517F-497D-9E68-C54C1E831665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0A6F9E39-FCA1-46E1-AACD-C11B965DCF3E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>aluno</t>
   </si>
@@ -64,39 +64,6 @@
   </si>
   <si>
     <t>Leandra Rabello</t>
-  </si>
-  <si>
-    <t>5,6</t>
-  </si>
-  <si>
-    <t>7,2</t>
-  </si>
-  <si>
-    <t>8,6</t>
-  </si>
-  <si>
-    <t>9,5</t>
-  </si>
-  <si>
-    <t>5,9</t>
-  </si>
-  <si>
-    <t>8,5</t>
-  </si>
-  <si>
-    <t>6,7</t>
-  </si>
-  <si>
-    <t>6,9</t>
-  </si>
-  <si>
-    <t>8,7</t>
-  </si>
-  <si>
-    <t>7,9</t>
-  </si>
-  <si>
-    <t>5,8</t>
   </si>
 </sst>
 </file>
@@ -449,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487AE2B3-2A40-4431-87CD-F17820C46026}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,31 +454,31 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>5.6</v>
       </c>
       <c r="C2">
         <v>6.7</v>
       </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" t="s">
-        <v>23</v>
+      <c r="D2">
+        <v>6.7</v>
+      </c>
+      <c r="E2">
+        <v>5.8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3">
+        <v>7.2</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>20</v>
+      <c r="D3">
+        <v>6.7</v>
       </c>
       <c r="E3">
         <v>9</v>
@@ -524,14 +491,14 @@
       <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
+      <c r="C4">
+        <v>5.9</v>
+      </c>
+      <c r="D4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E4">
+        <v>6.9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -544,10 +511,10 @@
       <c r="C5">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
+      <c r="D5">
+        <v>5.6</v>
+      </c>
+      <c r="E5" s="1">
         <v>7</v>
       </c>
     </row>
@@ -555,14 +522,14 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
+      <c r="B6">
+        <v>8.6</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>22</v>
+      <c r="D6">
+        <v>7.9</v>
       </c>
       <c r="E6">
         <v>8</v>
@@ -572,11 +539,11 @@
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
+      <c r="B7">
+        <v>9.5</v>
+      </c>
+      <c r="C7">
+        <v>8.5</v>
       </c>
       <c r="D7">
         <v>9</v>
@@ -584,9 +551,6 @@
       <c r="E7">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>